<commit_message>
corrected some bugs in variable names, and start reading crop management
</commit_message>
<xml_diff>
--- a/input/SimulationOptions.xlsx
+++ b/input/SimulationOptions.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="1040" windowWidth="22740" windowHeight="10860" tabRatio="500"/>
+    <workbookView xWindow="3680" yWindow="5300" windowWidth="22740" windowHeight="10860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="generalOptions" sheetId="1" r:id="rId1"/>
     <sheet name="cases" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>simustart</t>
   </si>
@@ -71,6 +71,30 @@
   </si>
   <si>
     <t>as.Date</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>management</t>
+  </si>
+  <si>
+    <t>"MAIZE.bidule"</t>
+  </si>
+  <si>
+    <t>"Chickpea.Ghab2", "WHEAT.Cocorit", "WHEAT.Avoine_Romani"</t>
+  </si>
+  <si>
+    <t>"ROTATION_BLE", "ROTATION_BLE_IRRIGUE"</t>
+  </si>
+  <si>
+    <t>"Gorgan-RFD"</t>
+  </si>
+  <si>
+    <t>"ROTATION_POISCHICHE", "ROTATION_BLE", "ROTATION_BLE_IRRIGUE"</t>
+  </si>
+  <si>
+    <t>"WHEAT.Ble_Dur_1", "WHEAT.Ble_Tendre_1"</t>
   </si>
 </sst>
 </file>
@@ -470,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -516,18 +540,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -543,8 +568,14 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -560,8 +591,14 @@
       <c r="E2">
         <v>-5</v>
       </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -577,8 +614,14 @@
       <c r="E3">
         <v>-5</v>
       </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -593,6 +636,12 @@
       </c>
       <c r="E4">
         <v>-5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all options for sowing finished !
the scenarios of crop rotations and crop management are read from excel file SimulationOptions.xlsx
Maize still produces bugs
I haven't yet coded harvest so there is still no rotation of crops.
</commit_message>
<xml_diff>
--- a/input/SimulationOptions.xlsx
+++ b/input/SimulationOptions.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="5300" windowWidth="22740" windowHeight="10860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13360" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="generalOptions" sheetId="1" r:id="rId1"/>
-    <sheet name="cases" sheetId="2" r:id="rId2"/>
+    <sheet name="cases_doesn't work" sheetId="2" r:id="rId2"/>
+    <sheet name="cases" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>simustart</t>
   </si>
@@ -95,6 +96,9 @@
   </si>
   <si>
     <t>"WHEAT.Ble_Dur_1", "WHEAT.Ble_Tendre_1"</t>
+  </si>
+  <si>
+    <t>this simulation set does not work because there are still bugs with maize appearing on day 256</t>
   </si>
 </sst>
 </file>
@@ -150,8 +154,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -160,9 +166,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,10 +548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -644,6 +652,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -653,4 +666,93 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>35</v>
+      </c>
+      <c r="E2">
+        <v>-5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>-5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected the bug on maize photoperiod response
now all three crops run !
</commit_message>
<xml_diff>
--- a/input/SimulationOptions.xlsx
+++ b/input/SimulationOptions.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13360" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="generalOptions" sheetId="1" r:id="rId1"/>
-    <sheet name="cases_doesn't work" sheetId="2" r:id="rId2"/>
-    <sheet name="cases" sheetId="3" r:id="rId3"/>
+    <sheet name="cases" sheetId="2" r:id="rId2"/>
+    <sheet name="caseswithoutmaize" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>simustart</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>"WHEAT.Ble_Dur_1", "WHEAT.Ble_Tendre_1"</t>
-  </si>
-  <si>
-    <t>this simulation set does not work because there are still bugs with maize appearing on day 256</t>
   </si>
 </sst>
 </file>
@@ -548,10 +545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -650,11 +647,6 @@
       </c>
       <c r="G4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -672,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated documentation and climates
</commit_message>
<xml_diff>
--- a/input/SimulationOptions.xlsx
+++ b/input/SimulationOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achille\Documents\GitHub\SSM.R\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13297BCE-F326-4B6C-A42E-144FFA66FB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF923F78-1FF2-417E-AB00-C4CB2A72D6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,17 @@
     <sheet name="caseswithoutmaize" sheetId="3" r:id="rId3"/>
     <sheet name="cases" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -105,9 +114,6 @@
     <t>"WHEAT.Ble_Dur_1", "WHEAT.Ble_Tendre_1"</t>
   </si>
   <si>
-    <t>"WHEAT.Ble_Dur_1"</t>
-  </si>
-  <si>
     <t>Turgutlu</t>
   </si>
   <si>
@@ -126,7 +132,10 @@
     <t>Meknes</t>
   </si>
   <si>
-    <t>"ROTATION_BLE_IRRIGUE"</t>
+    <t>"Chickpea.Ghab2"</t>
+  </si>
+  <si>
+    <t>"achille_rainfed_3N"</t>
   </si>
 </sst>
 </file>
@@ -597,7 +606,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -714,7 +723,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -803,7 +812,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -837,7 +846,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -852,7 +861,7 @@
         <v>-5.5049999999999999</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
@@ -860,10 +869,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -875,7 +884,7 @@
         <v>27.7288</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -883,10 +892,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -898,7 +907,7 @@
         <v>-5.7191000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -906,10 +915,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -921,7 +930,7 @@
         <v>4.0134999999999996</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
@@ -929,10 +938,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -944,7 +953,7 @@
         <v>9.7606999999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Revert "Updated documentation and climates"
This reverts commit 7d10944d51d7c67670a91cc0cd695d026b5dbcf8.
</commit_message>
<xml_diff>
--- a/input/SimulationOptions.xlsx
+++ b/input/SimulationOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achille\Documents\GitHub\SSM.R\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF923F78-1FF2-417E-AB00-C4CB2A72D6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13297BCE-F326-4B6C-A42E-144FFA66FB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,8 @@
     <sheet name="caseswithoutmaize" sheetId="3" r:id="rId3"/>
     <sheet name="cases" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140000"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -114,6 +105,9 @@
     <t>"WHEAT.Ble_Dur_1", "WHEAT.Ble_Tendre_1"</t>
   </si>
   <si>
+    <t>"WHEAT.Ble_Dur_1"</t>
+  </si>
+  <si>
     <t>Turgutlu</t>
   </si>
   <si>
@@ -132,10 +126,7 @@
     <t>Meknes</t>
   </si>
   <si>
-    <t>"Chickpea.Ghab2"</t>
-  </si>
-  <si>
-    <t>"achille_rainfed_3N"</t>
+    <t>"ROTATION_BLE_IRRIGUE"</t>
   </si>
 </sst>
 </file>
@@ -606,7 +597,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -723,7 +714,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -812,7 +803,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -846,7 +837,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -861,7 +852,7 @@
         <v>-5.5049999999999999</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
@@ -869,10 +860,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -884,7 +875,7 @@
         <v>27.7288</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -892,10 +883,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -907,7 +898,7 @@
         <v>-5.7191000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -915,10 +906,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -930,7 +921,7 @@
         <v>4.0134999999999996</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
@@ -938,10 +929,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -953,7 +944,7 @@
         <v>9.7606999999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Fixed rotations of crops
</commit_message>
<xml_diff>
--- a/input/SimulationOptions.xlsx
+++ b/input/SimulationOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achille\Documents\GitHub\SSM.R\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A4000F-CCBB-40DE-A228-F164BF80F28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C88A9D2-A8CC-4D8D-8F05-0284ACDFA87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>"WHEAT.Ble_Dur_1", "WHEAT.Ble_Tendre_1"</t>
   </si>
   <si>
-    <t>"WHEAT.Ble_Dur_1"</t>
-  </si>
-  <si>
     <t>Turgutlu</t>
   </si>
   <si>
@@ -126,7 +123,10 @@
     <t>Meknes</t>
   </si>
   <si>
-    <t>"achille_rainfed_3N"</t>
+    <t>c("achille_rainfed_3N","achille_rainfed_3N")</t>
+  </si>
+  <si>
+    <t>c("WHEAT.Ble_Dur_1", "Chickpea.Ghab2")</t>
   </si>
 </sst>
 </file>
@@ -803,13 +803,13 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -837,7 +837,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -852,18 +852,18 @@
         <v>-5.5049999999999999</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -875,18 +875,18 @@
         <v>27.7288</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -898,18 +898,18 @@
         <v>-5.7191000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -921,18 +921,18 @@
         <v>4.0134999999999996</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -944,10 +944,10 @@
         <v>9.7606999999999999</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Filters and debugging
</commit_message>
<xml_diff>
--- a/input/SimulationOptions.xlsx
+++ b/input/SimulationOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achille\Documents\GitHub\SSM.R\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4D763F-5F5A-4AED-9185-4E60B4EF1209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C88A9D2-A8CC-4D8D-8F05-0284ACDFA87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,8 @@
     <sheet name="caseswithoutmaize" sheetId="3" r:id="rId3"/>
     <sheet name="cases" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140000"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -132,10 +123,10 @@
     <t>Meknes</t>
   </si>
   <si>
-    <t>"achille_rainfed_3N"</t>
-  </si>
-  <si>
-    <t>"Chickpea.Ghab2"</t>
+    <t>c("achille_rainfed_3N","achille_rainfed_3N")</t>
+  </si>
+  <si>
+    <t>c("WHEAT.Ble_Dur_1", "Chickpea.Ghab2")</t>
   </si>
 </sst>
 </file>
@@ -723,7 +714,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -812,13 +803,13 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>